<commit_message>
updated 26/05/2024 23:33 GMT
</commit_message>
<xml_diff>
--- a/logbook.xlsx
+++ b/logbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Projects\Web\Python\Normal\logbook-data-science-artificial-intelligence-startup-campus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Projects\Python\logbook-data-science-artificial-intelligence-startup-campus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBAE3CB-5414-4172-8EE3-C01FC4152651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E814EE0-F9A8-4714-BF98-9E8B9CC5DD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="145">
   <si>
     <t>Date</t>
   </si>
@@ -903,10 +903,10 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q87" sqref="Q87"/>
+      <selection pane="bottomRight" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,7 +3793,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="2"/>
-      <c r="E87" s="12"/>
+      <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2" t="s">
         <v>102</v>
@@ -3811,9 +3811,7 @@
         <v>136</v>
       </c>
       <c r="P87" s="2"/>
-      <c r="Q87" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="Q87" s="12"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="3">

</xml_diff>

<commit_message>
updated 08/06/2024 16:21 WITA
</commit_message>
<xml_diff>
--- a/logbook.xlsx
+++ b/logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Projects\Python\logbook-data-science-artificial-intelligence-startup-campus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E814EE0-F9A8-4714-BF98-9E8B9CC5DD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FA8E6B-B7D6-4ED4-AB40-61D27B0D27FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -388,9 +388,6 @@
     <t>Generative AI: LLM and LVM</t>
   </si>
   <si>
-    <t>Konsultasi Final Project Tambahan</t>
-  </si>
-  <si>
     <t>Quiz 10 Learning Video</t>
   </si>
   <si>
@@ -412,12 +409,6 @@
     <t>MSIB | Kenali Kebutuhan Diri Menjaga Pikiran dan Hati</t>
   </si>
   <si>
-    <t>Be a Better You</t>
-  </si>
-  <si>
-    <t>Final Chapter</t>
-  </si>
-  <si>
     <t>Communication for Collaboration: Your Guide for Better Connection</t>
   </si>
   <si>
@@ -448,9 +439,6 @@
     <t>Onboarding &amp;&amp;&amp; Fun Day &amp;&amp;&amp; Graduation</t>
   </si>
   <si>
-    <t>Final Project Milestone &amp;&amp;&amp; Showcase Series</t>
-  </si>
-  <si>
     <t>Assignment Career &amp;&amp;&amp; Assignment Personal Branding</t>
   </si>
   <si>
@@ -461,6 +449,27 @@
   </si>
   <si>
     <t>2nd Checking Point: Monthly Reflection</t>
+  </si>
+  <si>
+    <t>Technical Meeting Selection to Showcase Data Science &amp; Artificial Intelligence Batch 6</t>
+  </si>
+  <si>
+    <t>Final Project Kick Off &amp;&amp;&amp; Final Project Milestone &amp;&amp;&amp; Showcase Series</t>
+  </si>
+  <si>
+    <t>Kick Off Final Project Data Science &amp; AI Batch 6</t>
+  </si>
+  <si>
+    <t>Student Journey MSIB 6 Be a Better You</t>
+  </si>
+  <si>
+    <t>Finalist Announcement</t>
+  </si>
+  <si>
+    <t>Diskusi mengenai KRS oleh Dosen Pembimbing Program MSIB Batch 6</t>
+  </si>
+  <si>
+    <t>Bimtek Penyusunan Laporan Akhir Mahasiswa MSIB Angkatan 6</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,12 +515,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,14 +609,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -906,7 +908,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F99" sqref="F99"/>
+      <selection pane="bottomRight" activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,8 +922,8 @@
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
     <col min="8" max="8" width="166.140625" customWidth="1"/>
     <col min="9" max="9" width="59.5703125" customWidth="1"/>
-    <col min="10" max="10" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="94.140625" customWidth="1"/>
+    <col min="11" max="11" width="69" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="122.42578125" customWidth="1"/>
@@ -958,25 +960,25 @@
         <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>67</v>
@@ -1009,7 +1011,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1807,7 +1809,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="9"/>
+      <c r="G27" s="8"/>
       <c r="H27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1838,10 +1840,10 @@
         <v>2</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -1873,12 +1875,12 @@
       <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -1906,10 +1908,10 @@
         <v>2</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -1941,10 +1943,10 @@
       <c r="D31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -1972,10 +1974,10 @@
         <v>2</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -2003,7 +2005,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>99</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -2083,7 +2085,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2218,7 +2220,7 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2271,7 +2273,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
@@ -2418,7 +2420,7 @@
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
@@ -2667,7 +2669,7 @@
         <v>114</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
@@ -2781,7 +2783,7 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -2840,7 +2842,7 @@
         <v>42</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="K58" s="2"/>
       <c r="L58" s="2" t="s">
@@ -2892,7 +2894,7 @@
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -2927,7 +2929,7 @@
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -2953,14 +2955,14 @@
       <c r="J61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K61" s="11"/>
+      <c r="K61" s="10"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
       <c r="Q61" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -2974,7 +2976,7 @@
         <v>3</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -2988,14 +2990,14 @@
       <c r="J62" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K62" s="11"/>
+      <c r="K62" s="10"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -3021,7 +3023,7 @@
       <c r="J63" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K63" s="11"/>
+      <c r="K63" s="10"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2" t="s">
@@ -3030,7 +3032,7 @@
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -3054,14 +3056,14 @@
       <c r="J64" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K64" s="11"/>
+      <c r="K64" s="10"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
       <c r="Q64" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -3075,7 +3077,7 @@
         <v>3</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2" t="s">
@@ -3088,7 +3090,7 @@
         <v>44</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -3096,7 +3098,7 @@
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
       <c r="Q65" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -3119,7 +3121,7 @@
         <v>44</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
@@ -3127,7 +3129,7 @@
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
       <c r="Q66" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -3150,7 +3152,7 @@
         <v>44</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>70</v>
@@ -3160,7 +3162,7 @@
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -3183,7 +3185,7 @@
         <v>44</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
@@ -3191,7 +3193,7 @@
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -3205,7 +3207,7 @@
         <v>3</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -3218,7 +3220,7 @@
         <v>44</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
@@ -3228,7 +3230,7 @@
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -3251,7 +3253,7 @@
         <v>45</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -3261,7 +3263,7 @@
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -3275,7 +3277,7 @@
         <v>3</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
@@ -3288,7 +3290,7 @@
         <v>45</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -3296,7 +3298,7 @@
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
       <c r="Q71" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -3321,7 +3323,7 @@
         <v>45</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -3329,7 +3331,7 @@
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
       <c r="Q72" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -3360,7 +3362,7 @@
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -3374,7 +3376,7 @@
         <v>3</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -3393,7 +3395,7 @@
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -3424,7 +3426,7 @@
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
       <c r="Q75" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -3455,7 +3457,7 @@
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -3469,11 +3471,11 @@
         <v>3</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -3490,7 +3492,7 @@
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
       <c r="Q77" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -3521,7 +3523,7 @@
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -3549,9 +3551,7 @@
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
-      <c r="Q79" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q79" s="2"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
@@ -3564,7 +3564,7 @@
         <v>4</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -3579,12 +3579,10 @@
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P80" s="2"/>
-      <c r="Q80" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q80" s="2"/>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
@@ -3612,12 +3610,10 @@
         <v>66</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P81" s="2"/>
-      <c r="Q81" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q81" s="2"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
@@ -3641,16 +3637,14 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P82" s="2"/>
-      <c r="Q82" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q82" s="2"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
@@ -3663,7 +3657,7 @@
         <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
@@ -3680,12 +3674,10 @@
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P83" s="2"/>
-      <c r="Q83" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q83" s="2"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
@@ -3711,12 +3703,10 @@
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P84" s="2"/>
-      <c r="Q84" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q84" s="2"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
@@ -3742,12 +3732,10 @@
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P85" s="2"/>
-      <c r="Q85" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q85" s="2"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
@@ -3760,7 +3748,7 @@
         <v>4</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -3775,12 +3763,10 @@
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
       <c r="O86" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P86" s="2"/>
-      <c r="Q86" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="Q86" s="2"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
@@ -3808,10 +3794,10 @@
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P87" s="2"/>
-      <c r="Q87" s="12"/>
+      <c r="Q87" s="2"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
@@ -3824,13 +3810,9 @@
         <v>4</v>
       </c>
       <c r="D88" s="2"/>
-      <c r="E88" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E88" s="2"/>
       <c r="F88" s="2"/>
-      <c r="G88" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2" t="s">
@@ -3842,9 +3824,7 @@
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
-      <c r="Q88" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="Q88" s="2"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
@@ -3857,17 +3837,13 @@
         <v>4</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>120</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G89" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2" t="s">
@@ -3879,9 +3855,7 @@
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
-      <c r="Q89" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="Q89" s="2"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
@@ -3894,13 +3868,9 @@
         <v>4</v>
       </c>
       <c r="D90" s="2"/>
-      <c r="E90" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2" t="s">
@@ -3912,9 +3882,7 @@
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
-      <c r="Q90" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="Q90" s="2"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
@@ -3927,13 +3895,9 @@
         <v>4</v>
       </c>
       <c r="D91" s="2"/>
-      <c r="E91" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2" t="s">
@@ -3945,9 +3909,7 @@
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
       <c r="P91" s="2"/>
-      <c r="Q91" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="Q91" s="2"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
@@ -3960,13 +3922,11 @@
         <v>4</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>120</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E92" s="2"/>
       <c r="F92" s="2"/>
-      <c r="G92" s="6" t="s">
+      <c r="G92" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H92" s="2"/>
@@ -3980,8 +3940,8 @@
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
       <c r="P92" s="2"/>
-      <c r="Q92" s="6" t="s">
-        <v>128</v>
+      <c r="Q92" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
@@ -3995,13 +3955,9 @@
         <v>4</v>
       </c>
       <c r="D93" s="2"/>
-      <c r="E93" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E93" s="2"/>
       <c r="F93" s="2"/>
-      <c r="G93" s="6" t="s">
-        <v>103</v>
-      </c>
+      <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2" t="s">
@@ -4013,9 +3969,7 @@
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
       <c r="P93" s="2"/>
-      <c r="Q93" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q93" s="2"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
@@ -4028,9 +3982,7 @@
         <v>4</v>
       </c>
       <c r="D94" s="2"/>
-      <c r="E94" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -4038,7 +3990,7 @@
         <v>49</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
@@ -4046,9 +3998,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
-      <c r="Q94" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q94" s="2"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
@@ -4061,11 +4011,9 @@
         <v>4</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>120</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E95" s="2"/>
       <c r="F95" s="2" t="s">
         <v>27</v>
       </c>
@@ -4083,9 +4031,7 @@
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
-      <c r="Q95" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q95" s="2"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
@@ -4098,9 +4044,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="2"/>
-      <c r="E96" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -4116,9 +4060,7 @@
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
-      <c r="Q96" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q96" s="2"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
@@ -4131,9 +4073,7 @@
         <v>4</v>
       </c>
       <c r="D97" s="2"/>
-      <c r="E97" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -4143,15 +4083,15 @@
       <c r="J97" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K97" s="2"/>
+      <c r="K97" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
-      <c r="Q97" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q97" s="2"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
@@ -4164,11 +4104,9 @@
         <v>4</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>120</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -4184,9 +4122,7 @@
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
-      <c r="Q98" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q98" s="2"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
@@ -4199,17 +4135,13 @@
         <v>4</v>
       </c>
       <c r="D99" s="2"/>
-      <c r="E99" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
-      <c r="I99" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="I99" s="2"/>
       <c r="J99" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
@@ -4217,8 +4149,8 @@
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
-      <c r="Q99" s="6" t="s">
-        <v>129</v>
+      <c r="Q99" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -4237,9 +4169,7 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
-      <c r="J100" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="J100" s="2"/>
       <c r="K100" s="2" t="s">
         <v>52</v>
       </c>
@@ -4248,9 +4178,7 @@
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
-      <c r="Q100" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q100" s="2"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
@@ -4268,9 +4196,7 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
-      <c r="J101" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="J101" s="2"/>
       <c r="K101" s="2" t="s">
         <v>52</v>
       </c>
@@ -4279,9 +4205,7 @@
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
-      <c r="Q101" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q101" s="2"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
@@ -4300,7 +4224,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>52</v>
@@ -4310,9 +4234,7 @@
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
-      <c r="Q102" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q102" s="2"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
@@ -4330,9 +4252,7 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="J103" s="2"/>
       <c r="K103" s="2" t="s">
         <v>52</v>
       </c>
@@ -4341,9 +4261,7 @@
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
-      <c r="Q103" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q103" s="2"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
@@ -4361,9 +4279,7 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="J104" s="2"/>
       <c r="K104" s="2" t="s">
         <v>52</v>
       </c>
@@ -4372,9 +4288,7 @@
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
-      <c r="Q104" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q104" s="2"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
@@ -4393,7 +4307,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>52</v>
@@ -4403,9 +4317,7 @@
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
-      <c r="Q105" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q105" s="2"/>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
@@ -4424,19 +4336,15 @@
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
-      <c r="K106" s="6" t="s">
-        <v>134</v>
+      <c r="K106" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L106" s="2"/>
-      <c r="M106" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="M106" s="2"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
-      <c r="Q106" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q106" s="2"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
@@ -4455,19 +4363,15 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
-      <c r="K107" s="6" t="s">
-        <v>134</v>
+      <c r="K107" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L107" s="2"/>
-      <c r="M107" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="M107" s="2"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
-      <c r="Q107" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q107" s="2"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
@@ -4486,19 +4390,15 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
-      <c r="K108" s="6" t="s">
-        <v>134</v>
+      <c r="K108" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L108" s="2"/>
-      <c r="M108" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="M108" s="2"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>
-      <c r="Q108" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q108" s="2"/>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
@@ -4517,8 +4417,8 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
-      <c r="K109" s="6" t="s">
-        <v>134</v>
+      <c r="K109" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="L109" s="2"/>
       <c r="M109" s="2" t="s">
@@ -4527,9 +4427,7 @@
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
       <c r="P109" s="2"/>
-      <c r="Q109" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q109" s="2"/>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
@@ -4548,19 +4446,15 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
-      <c r="K110" s="6" t="s">
-        <v>134</v>
+      <c r="K110" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L110" s="2"/>
-      <c r="M110" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="M110" s="2"/>
       <c r="N110" s="2"/>
       <c r="O110" s="2"/>
       <c r="P110" s="2"/>
-      <c r="Q110" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q110" s="2"/>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
@@ -4579,19 +4473,15 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
-      <c r="K111" s="6" t="s">
-        <v>134</v>
+      <c r="K111" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="L111" s="2"/>
-      <c r="M111" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
-      <c r="Q111" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q111" s="2"/>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
@@ -4611,16 +4501,14 @@
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
       <c r="P112" s="2"/>
-      <c r="Q112" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q112" s="2"/>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
@@ -4640,16 +4528,14 @@
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
       <c r="P113" s="2"/>
-      <c r="Q113" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q113" s="2"/>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
@@ -4669,16 +4555,14 @@
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
       <c r="O114" s="2"/>
       <c r="P114" s="2"/>
-      <c r="Q114" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q114" s="2"/>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
@@ -4698,16 +4582,14 @@
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
       <c r="P115" s="2"/>
-      <c r="Q115" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q115" s="2"/>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
@@ -4727,16 +4609,14 @@
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
       <c r="P116" s="2"/>
-      <c r="Q116" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q116" s="2"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
@@ -4756,16 +4636,14 @@
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
       <c r="K117" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
-      <c r="Q117" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="Q117" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4779,7 +4657,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4915,7 +4793,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>75</v>
@@ -4934,22 +4812,22 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="11" t="b">
+      <c r="C8" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="11" t="b">
+      <c r="D8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4975,7 +4853,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>75</v>
@@ -4994,28 +4872,28 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="11" t="b">
+      <c r="C11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>74</v>
@@ -5035,7 +4913,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
updated 15/06/2024 15:26 WITA
</commit_message>
<xml_diff>
--- a/logbook.xlsx
+++ b/logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Projects\Python\logbook-data-science-artificial-intelligence-startup-campus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FA8E6B-B7D6-4ED4-AB40-61D27B0D27FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B14224-8C01-469B-BD72-46680A764A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="149">
   <si>
     <t>Date</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>Bimtek Penyusunan Laporan Akhir Mahasiswa MSIB Angkatan 6</t>
+  </si>
+  <si>
+    <t>Survei Akhir Kegiatan Program MSIB Angkatan 6 Tahun 2024 (Untuk Mahasiswa Studi Independen)</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -621,7 +624,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,10 +907,10 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H77" sqref="H77"/>
+      <selection pane="bottomRight" activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +931,7 @@
     <col min="14" max="14" width="122.42578125" customWidth="1"/>
     <col min="15" max="15" width="81" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="94.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="103.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="103.85546875" customWidth="1"/>
     <col min="18" max="23" width="9" customWidth="1"/>
     <col min="24" max="24" width="9.140625" customWidth="1"/>
   </cols>
@@ -3998,7 +4000,9 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
-      <c r="Q94" s="2"/>
+      <c r="Q94" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
@@ -4031,7 +4035,9 @@
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
-      <c r="Q95" s="2"/>
+      <c r="Q95" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
@@ -4060,7 +4066,9 @@
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
-      <c r="Q96" s="2"/>
+      <c r="Q96" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
@@ -4091,7 +4099,9 @@
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
-      <c r="Q97" s="2"/>
+      <c r="Q97" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
@@ -4122,7 +4132,9 @@
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
-      <c r="Q98" s="2"/>
+      <c r="Q98" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
@@ -4178,7 +4190,9 @@
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
-      <c r="Q100" s="2"/>
+      <c r="Q100" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
@@ -4205,7 +4219,9 @@
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
-      <c r="Q101" s="2"/>
+      <c r="Q101" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
@@ -4234,7 +4250,9 @@
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
-      <c r="Q102" s="2"/>
+      <c r="Q102" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
@@ -4261,7 +4279,9 @@
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
-      <c r="Q103" s="2"/>
+      <c r="Q103" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
@@ -4288,7 +4308,9 @@
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
-      <c r="Q104" s="2"/>
+      <c r="Q104" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
@@ -4317,7 +4339,9 @@
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
-      <c r="Q105" s="2"/>
+      <c r="Q105" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
@@ -4417,7 +4441,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
-      <c r="K109" s="11" t="s">
+      <c r="K109" s="2" t="s">
         <v>131</v>
       </c>
       <c r="L109" s="2"/>
@@ -4643,7 +4667,7 @@
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
-      <c r="Q117" s="11"/>
+      <c r="Q117" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>